<commit_message>
content-based ,cf model, azure function, expo go done
</commit_message>
<xml_diff>
--- a/Ressource/Avancement.xlsx
+++ b/Ressource/Avancement.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OpenClassroom_projet\Projet_9\Ressource\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FB6D224-42BE-44BB-87E8-742277F939CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D121089-9F62-410C-BD5F-C3BB77985006}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t xml:space="preserve">Tache à réaliser : </t>
   </si>
@@ -79,18 +79,6 @@
   </si>
   <si>
     <t>les scripts sont stockés dans un dossier GitHub</t>
-  </si>
-  <si>
-    <t>Début des recherches</t>
-  </si>
-  <si>
-    <t>Azure function (serverless) -&gt; Mobile App</t>
-  </si>
-  <si>
-    <t>Création faite plus qu'a push</t>
-  </si>
-  <si>
-    <t>Récupération des fichier uniquement pour le moment</t>
   </si>
 </sst>
 </file>
@@ -682,7 +670,7 @@
   <dimension ref="B2:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -716,7 +704,7 @@
       <c r="D4" s="6"/>
       <c r="F4" s="3">
         <f>AVERAGE(C5:C8,C10:C14)</f>
-        <v>0.23333333333333334</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="2:7" ht="56.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -726,16 +714,14 @@
       <c r="C5" s="9">
         <v>1</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>16</v>
-      </c>
+      <c r="D5" s="5"/>
     </row>
     <row r="6" spans="2:7" ht="56.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="9">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="D6" s="5"/>
     </row>
@@ -744,7 +730,7 @@
         <v>7</v>
       </c>
       <c r="C7" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7" s="4"/>
     </row>
@@ -753,7 +739,7 @@
         <v>8</v>
       </c>
       <c r="C8" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8" s="14"/>
     </row>
@@ -769,18 +755,16 @@
         <v>10</v>
       </c>
       <c r="C10" s="9">
-        <v>0.1</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>15</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="D10" s="5"/>
     </row>
     <row r="11" spans="2:7" ht="53.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C11" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11" s="5"/>
       <c r="G11" s="13"/>
@@ -790,7 +774,7 @@
         <v>12</v>
       </c>
       <c r="C12" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D12" s="5"/>
     </row>
@@ -799,22 +783,18 @@
         <v>13</v>
       </c>
       <c r="C13" s="9">
-        <v>0.3</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>18</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="D13" s="5"/>
     </row>
     <row r="14" spans="2:7" ht="83" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C14" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>17</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="D14" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>